<commit_message>
Incorporate recent 3.0 edits from US EPS
</commit_message>
<xml_diff>
--- a/InputData/trans/PCiCDTdtTDM/Perc Chng in Cargo Dist Transported due to TDM.xlsx
+++ b/InputData/trans/PCiCDTdtTDM/Perc Chng in Cargo Dist Transported due to TDM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\trans\PCiCDTdtTDM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-minnesota\InputData\trans\PCiCDTdtTDM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
   <si>
     <t>Source:</t>
   </si>
@@ -261,6 +261,9 @@
   </si>
   <si>
     <t>Percent Change (dimensionless)</t>
+  </si>
+  <si>
+    <t>We allow for twice the potential identified in the BLUE Shifts scenario.</t>
   </si>
 </sst>
 </file>
@@ -361,11 +364,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -815,18 +818,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -834,168 +839,173 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" s="2">
         <v>2009</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A43" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1014,36 +1024,36 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.1328125" customWidth="1"/>
+    <col min="2" max="2" width="18.3984375" customWidth="1"/>
+    <col min="3" max="3" width="16.73046875" customWidth="1"/>
+    <col min="4" max="4" width="13.73046875" customWidth="1"/>
+    <col min="5" max="5" width="11.3984375" customWidth="1"/>
+    <col min="8" max="8" width="14.73046875" customWidth="1"/>
+    <col min="10" max="10" width="14.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B3" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>24</v>
       </c>
@@ -1075,7 +1085,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
@@ -1108,7 +1118,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
@@ -1156,33 +1166,33 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.3984375" customWidth="1"/>
+    <col min="2" max="2" width="14.3984375" customWidth="1"/>
+    <col min="3" max="3" width="16.1328125" customWidth="1"/>
+    <col min="4" max="4" width="17.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B3" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>24</v>
       </c>
@@ -1204,7 +1214,7 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
@@ -1226,7 +1236,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
@@ -1263,19 +1273,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="29.59765625" customWidth="1"/>
+    <col min="2" max="2" width="15.73046875" customWidth="1"/>
+    <col min="7" max="7" width="16.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>24</v>
       </c>
@@ -1301,7 +1311,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>25</v>
       </c>
@@ -1333,7 +1343,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>26</v>
       </c>
@@ -1365,7 +1375,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>42</v>
       </c>
@@ -1397,12 +1407,12 @@
         <v>-0.15257731958762888</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
@@ -1416,7 +1426,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
         <v>25</v>
       </c>
@@ -1433,7 +1443,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>26</v>
       </c>
@@ -1450,7 +1460,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
         <v>42</v>
       </c>
@@ -1482,17 +1492,19 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.59765625" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="13" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="9" t="s">
@@ -1502,75 +1514,75 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="8">
-        <f>Calcs!B5</f>
-        <v>-0.26013513513513514</v>
+        <f>Calcs!B5*2</f>
+        <v>-0.52027027027027029</v>
       </c>
       <c r="C2" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="8">
-        <f>Calcs!C5</f>
-        <v>0.61764705882352944</v>
+        <f>Calcs!C5*2</f>
+        <v>1.2352941176470589</v>
       </c>
       <c r="C3" s="8">
-        <f>Calcs!B11</f>
-        <v>-0.17518248175182483</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <f>Calcs!B11*2</f>
+        <v>-0.35036496350364965</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>39</v>
       </c>
       <c r="B4" s="8">
-        <f>Calcs!D5</f>
-        <v>-0.29850746268656714</v>
+        <f>Calcs!D5*2</f>
+        <v>-0.59701492537313428</v>
       </c>
       <c r="C4" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>40</v>
       </c>
       <c r="B5" s="8">
-        <f>Calcs!E5</f>
-        <v>1.0476190476190477</v>
+        <f>Calcs!E5*2</f>
+        <v>2.0952380952380953</v>
       </c>
       <c r="C5" s="8">
-        <f>Calcs!C11</f>
-        <v>0.12686567164179105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <f>Calcs!C11*2</f>
+        <v>0.2537313432835821</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>41</v>
       </c>
       <c r="B6">
-        <f>Calcs!F5</f>
+        <f>Calcs!F5*2</f>
         <v>0</v>
       </c>
       <c r="C6" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>50</v>
       </c>
       <c r="B7">
-        <f>Calcs!G5</f>
-        <v>-0.5</v>
+        <f>Calcs!G5*2</f>
+        <v>-1</v>
       </c>
       <c r="C7" s="10">
         <v>0</v>

</xml_diff>